<commit_message>
CP033688 para sheep addition
</commit_message>
<xml_diff>
--- a/dependencies/bi/salmonella/typhimurium-LT2/script_dependents/RemoveFromAnalysis.xlsx
+++ b/dependencies/bi/salmonella/typhimurium-LT2/script_dependents/RemoveFromAnalysis.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/root/TStuber/Results/gen-bact/salmonella/typhimurium/script_dependents/script2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\TStuber\Results\bi\salmonella\vsnp\typhimurium-LT2\script_dependents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EFB369E1-58A4-A448-8412-629B40CBA2F3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68360" yWindow="9220" windowWidth="21040" windowHeight="14740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68364" yWindow="9216" windowWidth="21036" windowHeight="14736" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,11 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>18-012180-417</t>
+  </si>
+  <si>
+    <t>18-006979-297</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -39,12 +45,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -59,9 +71,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,18 +354,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="46.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.796875" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>